<commit_message>
excel con tablas updated!
</commit_message>
<xml_diff>
--- a/tabla de triggers.xlsx
+++ b/tabla de triggers.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="23256" windowHeight="12072"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="19440" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="75">
   <si>
     <t>i</t>
   </si>
@@ -60,9 +60,6 @@
     <t>Goles</t>
   </si>
   <si>
-    <t>estado=iniciado</t>
-  </si>
-  <si>
     <t>solamente si estado = iniciado</t>
   </si>
   <si>
@@ -151,13 +148,106 @@
   </si>
   <si>
     <t>no se puede si fecha no coincide con ultima ronda</t>
+  </si>
+  <si>
+    <t>estado=inicio</t>
+  </si>
+  <si>
+    <t>no se puede agregar un torneo si otro torneo tiene estado de iniciado o en proceso</t>
+  </si>
+  <si>
+    <t>no se puede cambiar la cancha</t>
+  </si>
+  <si>
+    <t>calendario</t>
+  </si>
+  <si>
+    <t>a menos que este no se hayan jugado todavia los partidos</t>
+  </si>
+  <si>
+    <t>no pueden haber lugares iguales con la misma hora</t>
+  </si>
+  <si>
+    <t>torneo</t>
+  </si>
+  <si>
+    <t>partido</t>
+  </si>
+  <si>
+    <t>update no se puede si es en otra fecha_actual</t>
+  </si>
+  <si>
+    <t>no puede cambar id_calendario</t>
+  </si>
+  <si>
+    <t>fecha no se puede cambiar si es que es una anterior a fecha_actul de torneo</t>
+  </si>
+  <si>
+    <t>cancha</t>
+  </si>
+  <si>
+    <t>equipo</t>
+  </si>
+  <si>
+    <t>no se puede update el id</t>
+  </si>
+  <si>
+    <t>no se puede cambiar el id</t>
+  </si>
+  <si>
+    <t>no puede repetirse el nombre</t>
+  </si>
+  <si>
+    <t>goles_x_jugador</t>
+  </si>
+  <si>
+    <t>solo se puede cambiar a favor y en contra</t>
+  </si>
+  <si>
+    <t>en la fecha que se jugo ese partido</t>
+  </si>
+  <si>
+    <t>jugador</t>
+  </si>
+  <si>
+    <t>solo se puede cambiar si torneo esta en inicio</t>
+  </si>
+  <si>
+    <t>no se puede cambiar id ni ronda</t>
+  </si>
+  <si>
+    <t>no se puede cambiar nada!!!</t>
+  </si>
+  <si>
+    <t>planilla</t>
+  </si>
+  <si>
+    <t>no se puede cambiar id, id partido, jugador, equipo</t>
+  </si>
+  <si>
+    <t>puede cambiar titular solamente si no se jugo todav</t>
+  </si>
+  <si>
+    <t>ronda</t>
+  </si>
+  <si>
+    <t>no se puede cambiar nada</t>
+  </si>
+  <si>
+    <t>tabla</t>
+  </si>
+  <si>
+    <t>no se puede cambiar id, equipo, anho</t>
+  </si>
+  <si>
+    <t>se puede cambiar posicion y puntaje</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -223,7 +313,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -297,7 +387,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -332,7 +421,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -508,25 +596,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.109375" customWidth="1"/>
-    <col min="3" max="3" width="22.88671875" customWidth="1"/>
-    <col min="4" max="4" width="56.5546875" customWidth="1"/>
-    <col min="5" max="5" width="27.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.109375" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" customWidth="1"/>
+    <col min="4" max="4" width="36.28515625" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8">
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
@@ -540,7 +628,7 @@
       </c>
       <c r="G1" s="4"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8">
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
@@ -560,256 +648,374 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="E3" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="H3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="H4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="E7" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="H8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="E9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="G9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" s="2" t="s">
+      <c r="G10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="E11" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>13</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C21" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
+        <v>67</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C22" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>70</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
+        <v>72</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C24" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -823,24 +1029,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
consistencia hasta la tabla de goles
no me esta funcionando porque le falta id_rondas a la tabla de partidos
</commit_message>
<xml_diff>
--- a/tabla de triggers.xlsx
+++ b/tabla de triggers.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="74">
   <si>
     <t>i</t>
   </si>
@@ -204,9 +204,6 @@
     <t>solo se puede cambiar a favor y en contra</t>
   </si>
   <si>
-    <t>en la fecha que se jugo ese partido</t>
-  </si>
-  <si>
     <t>jugador</t>
   </si>
   <si>
@@ -225,9 +222,6 @@
     <t>no se puede cambiar id, id partido, jugador, equipo</t>
   </si>
   <si>
-    <t>puede cambiar titular solamente si no se jugo todav</t>
-  </si>
-  <si>
     <t>ronda</t>
   </si>
   <si>
@@ -241,6 +235,9 @@
   </si>
   <si>
     <t>se puede cambiar posicion y puntaje</t>
+  </si>
+  <si>
+    <t>no se puede fuera de fecha</t>
   </si>
 </sst>
 </file>
@@ -256,7 +253,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -275,6 +272,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -288,7 +291,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -298,6 +301,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -600,7 +604,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -956,25 +960,25 @@
       </c>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="5" t="s">
         <v>60</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D19" t="s">
-        <v>62</v>
+      <c r="D19" s="2" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -982,40 +986,37 @@
         <v>51</v>
       </c>
       <c r="B21" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C21" t="s">
         <v>65</v>
-      </c>
-      <c r="C21" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
+        <v>66</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C22" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
+        <v>70</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C24" t="s">
         <v>72</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C24" t="s">
-        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>